<commit_message>
AI inside DX Suite OCR への対応
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\work\git\DocumentUnderstandingEvaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Source\Repos\DocumentUnderstandingEvaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06EA826-B85B-40B2-888C-5B85D72BC8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EECCE6A-292E-426D-A7DD-22DE6A53C8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="735" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="735" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSettings" sheetId="14" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="145">
   <si>
     <t>Name</t>
   </si>
@@ -579,6 +579,26 @@
   </si>
   <si>
     <t>The API key used to provide you access to the Cogent Labs SmartRead OCR.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>OCR_AIinsideOCR_Use</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>OCR_AIinsideOCR_ApiKey</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>The API key used to provide you access to the AI inside OCR.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>OCR_AIinsideOCR_EndPoint</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>The endpoint associated with your AI inside OCR API key. This field supports only strings and String variables.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1875,8 +1895,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{743D77D5-EAF3-4F4C-8A38-EEBDC77DFB2F}" name="OcrSettings" displayName="OcrSettings" ref="A1:F15" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:F15" xr:uid="{4176AEA8-5810-48C0-8FA3-12A94CAE1E54}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{743D77D5-EAF3-4F4C-8A38-EEBDC77DFB2F}" name="OcrSettings" displayName="OcrSettings" ref="A1:F19" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:F19" xr:uid="{4176AEA8-5810-48C0-8FA3-12A94CAE1E54}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{A2C6C8F3-7C23-4751-B4DC-97F344C08A77}" name="Name" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{C2D1B7CB-6985-4D52-BF49-16AD7AE7C283}" name="Value" dataDxfId="21"/>
@@ -2216,8 +2236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BCE469-BC90-4982-9CD3-7942BA4D4066}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2404,7 +2424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7BE991-0805-438E-A28D-2AC2A75CC1EB}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3013,11 +3033,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AEE009-FD56-4FA4-9E8D-0BF43DD91C81}">
-  <dimension ref="A1:AB15"/>
+  <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3288,30 +3306,90 @@
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="B1:B11 B15:B1048576">
+  <conditionalFormatting sqref="B1:B14 B19:B1048576">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>AND($B1="",$D1="Required")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:B14">
+  <conditionalFormatting sqref="B15:B18">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND($B12="",$D12="Required")</formula>
+      <formula>AND($B15="",$D15="Required")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:C7 B2:C2 B13:C13" xr:uid="{B817C909-71A7-4665-99E6-C80BF521D5EC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:C7 B2:C2 B13:C13 B16:C16" xr:uid="{B817C909-71A7-4665-99E6-C80BF521D5EC}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15" xr:uid="{2693A9CE-5134-404B-A5F2-2FC85632768C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D19" xr:uid="{2693A9CE-5134-404B-A5F2-2FC85632768C}">
       <formula1>"Required,Optional"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>